<commit_message>
create report audit log
</commit_message>
<xml_diff>
--- a/data/reporting/ROLE_MAPPING_OUTPUT_OF_TOOL_FOR_SECURITY.xlsx
+++ b/data/reporting/ROLE_MAPPING_OUTPUT_OF_TOOL_FOR_SECURITY.xlsx
@@ -120,9 +120,6 @@
     <t>Service Entry Sheet Creator</t>
   </si>
   <si>
-    <t>SRM Lead Requestor</t>
-  </si>
-  <si>
     <t>Stock Count Administrator</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>Purchasing Org</t>
+  </si>
+  <si>
+    <t>SRM Lead Requester</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,43 +814,43 @@
   <sheetData>
     <row r="1" spans="1:87" s="13" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>1</v>
@@ -880,13 +880,13 @@
         <v>30</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="Z1" s="7" t="s">
         <v>2</v>
@@ -895,16 +895,16 @@
         <v>28</v>
       </c>
       <c r="AB1" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE1" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF1" s="8" t="s">
         <v>20</v>
@@ -916,13 +916,13 @@
         <v>9</v>
       </c>
       <c r="AI1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="AK1" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AL1" s="8" t="s">
         <v>16</v>
@@ -937,13 +937,13 @@
         <v>5</v>
       </c>
       <c r="AP1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AR1" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="AR1" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="AS1" s="8" t="s">
         <v>15</v>
@@ -958,58 +958,58 @@
         <v>24</v>
       </c>
       <c r="AW1" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AX1" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AY1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BC1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="BE1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="BF1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="BG1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="BA1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BB1" s="9" t="s">
+      <c r="BI1" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="BC1" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="BD1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="BE1" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="BF1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="BH1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="BI1" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="BJ1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="BK1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="BL1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="BL1" s="9" t="s">
+      <c r="BM1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN1" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="BM1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="BN1" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="BO1" s="10" t="s">
         <v>11</v>
@@ -1024,46 +1024,46 @@
         <v>10</v>
       </c>
       <c r="BS1" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BT1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="BU1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="BV1" s="10" t="s">
+      <c r="BW1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="BW1" s="10" t="s">
+      <c r="BX1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="BY1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ1" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="BX1" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="BY1" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="BZ1" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="CA1" s="11" t="s">
         <v>22</v>
       </c>
       <c r="CB1" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CC1" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="CD1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="CE1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="CF1" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="CF1" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="CG1" s="7" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
retype mistake typo role in each report
</commit_message>
<xml_diff>
--- a/data/reporting/ROLE_MAPPING_OUTPUT_OF_TOOL_FOR_SECURITY.xlsx
+++ b/data/reporting/ROLE_MAPPING_OUTPUT_OF_TOOL_FOR_SECURITY.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
-    <t>AP Invoice Processor</t>
-  </si>
-  <si>
     <t>Backbone Reviewer/Approver</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>WM Mobile Technician</t>
   </si>
   <si>
-    <t>WM Microsoft Project (MSP)</t>
-  </si>
-  <si>
     <t>WM Occasional Work Request Creator</t>
   </si>
   <si>
@@ -274,6 +268,12 @@
   </si>
   <si>
     <t>Inventory Optimization Analyst</t>
+  </si>
+  <si>
+    <t>WM Microsoft Project</t>
+  </si>
+  <si>
+    <t>AP Invoice Processor  (GFT Job Role)</t>
   </si>
 </sst>
 </file>
@@ -790,10 +790,10 @@
   <dimension ref="A1:CI6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO6" sqref="AO6"/>
+      <selection pane="bottomRight" activeCell="BJ1" sqref="BJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,262 +817,262 @@
   <sheetData>
     <row r="1" spans="1:87" s="13" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="N1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="Y1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AU1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="6" t="s">
+      <c r="AY1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AZ1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="BA1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="BC1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="BE1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="BG1" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="BI1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BJ1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="BK1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="BN1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="BO1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="BP1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BQ1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="BT1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="BU1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="BV1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="BW1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="BX1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="BZ1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="CA1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="V1" s="7" t="s">
+      <c r="CB1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="CC1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="CD1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="CE1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="CF1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CG1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="CH1" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AO1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AS1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="AT1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="AU1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="AW1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="AY1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AZ1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="BA1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="BB1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="BC1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="BD1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="BE1" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="BF1" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="BG1" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="BH1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="BI1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="BJ1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="BK1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="BL1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="BM1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BN1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BO1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="BP1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="BQ1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="BR1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="BS1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="BU1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="BV1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="BW1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="BX1" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="BY1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="BZ1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="CA1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="CB1" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="CC1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="CD1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="CE1" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="CF1" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="CG1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="CH1" s="12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:87" s="3" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
update role to security report
</commit_message>
<xml_diff>
--- a/data/reporting/ROLE_MAPPING_OUTPUT_OF_TOOL_FOR_SECURITY.xlsx
+++ b/data/reporting/ROLE_MAPPING_OUTPUT_OF_TOOL_FOR_SECURITY.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$M$2:$CH$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$M$2:$CU$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>Backbone Reviewer/Approver</t>
   </si>
@@ -274,13 +274,52 @@
   </si>
   <si>
     <t>AP Invoice Processor  (GFT Job Role)</t>
+  </si>
+  <si>
+    <t>  Standard Desktop Confirmation Requester</t>
+  </si>
+  <si>
+    <t> Central Desktop Confirmation Requester</t>
+  </si>
+  <si>
+    <t>Strategic Materials Planner</t>
+  </si>
+  <si>
+    <t> Demand Planning MRP Specialist</t>
+  </si>
+  <si>
+    <t>Third Party Inventory Administrator</t>
+  </si>
+  <si>
+    <t>MDM - Local Data Steward</t>
+  </si>
+  <si>
+    <t>  VMI Administrator</t>
+  </si>
+  <si>
+    <t>Vendor Data Requestor (Egypt only)</t>
+  </si>
+  <si>
+    <t>MDM - Display</t>
+  </si>
+  <si>
+    <t>MDM - Global Data Steward</t>
+  </si>
+  <si>
+    <t>GWO Data Maintainer</t>
+  </si>
+  <si>
+    <t>  GWO Data Display</t>
+  </si>
+  <si>
+    <t>  Regional Maximo Labor Data Steward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,8 +360,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF500050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +420,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,11 +515,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -486,6 +547,19 @@
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,13 +861,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CI6"/>
+  <dimension ref="A1:CU6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BJ1" sqref="BJ1"/>
+      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,9 +878,9 @@
     <col min="4" max="4" width="3.28515625" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="4" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="12" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="12" width="5.140625" hidden="1" customWidth="1"/>
     <col min="13" max="36" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="38" max="48" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -815,359 +889,411 @@
     <col min="51" max="86" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="13" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:99" s="12" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AP1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AR1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AS1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AT1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AU1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AV1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AW1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AX1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AY1" s="9" t="s">
+      <c r="AY1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="BA1" s="9" t="s">
+      <c r="BA1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="BB1" s="9" t="s">
+      <c r="BB1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="BC1" s="9" t="s">
+      <c r="BC1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BD1" s="9" t="s">
+      <c r="BD1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="BE1" s="9" t="s">
+      <c r="BE1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="BF1" s="9" t="s">
+      <c r="BF1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="BG1" s="9" t="s">
+      <c r="BG1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BH1" s="9" t="s">
+      <c r="BH1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="BI1" s="9" t="s">
+      <c r="BI1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="BJ1" s="9" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="BK1" s="9" t="s">
+      <c r="BK1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="BL1" s="9" t="s">
+      <c r="BL1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="BM1" s="9" t="s">
+      <c r="BM1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="BN1" s="9" t="s">
+      <c r="BN1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="BO1" s="10" t="s">
+      <c r="BO1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BP1" s="10" t="s">
+      <c r="BP1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="BQ1" s="10" t="s">
+      <c r="BQ1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="BR1" s="10" t="s">
+      <c r="BR1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="BS1" s="10" t="s">
+      <c r="BS1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="BT1" s="10" t="s">
+      <c r="BT1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="BU1" s="10" t="s">
+      <c r="BU1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="BV1" s="10" t="s">
+      <c r="BV1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="BW1" s="10" t="s">
+      <c r="BW1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BX1" s="10" t="s">
+      <c r="BX1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="BY1" s="10" t="s">
+      <c r="BY1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="BZ1" s="10" t="s">
+      <c r="BZ1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="CA1" s="11" t="s">
+      <c r="CA1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="CB1" s="11" t="s">
+      <c r="CB1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="CC1" s="11" t="s">
+      <c r="CC1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="CD1" s="11" t="s">
+      <c r="CD1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="CE1" s="11" t="s">
+      <c r="CE1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="CF1" s="11" t="s">
+      <c r="CF1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="CG1" s="7" t="s">
+      <c r="CG1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="CH1" s="12" t="s">
+      <c r="CH1" s="11" t="s">
         <v>30</v>
       </c>
+      <c r="CI1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="CJ1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="CK1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="CL1" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="CM1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="CN1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="CO1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="CP1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="CQ1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="CR1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="CS1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="CT1" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="13" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="2" spans="1:87" s="3" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1"/>
-      <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="1"/>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="1"/>
-      <c r="BC2" s="1"/>
-      <c r="BD2" s="1"/>
-      <c r="BE2" s="1"/>
-      <c r="BF2" s="1"/>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="1"/>
-      <c r="BI2" s="1"/>
-      <c r="BJ2" s="1"/>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="1"/>
-      <c r="BN2" s="1"/>
-      <c r="BO2" s="1"/>
-      <c r="BP2" s="1"/>
-      <c r="BQ2" s="1"/>
-      <c r="BR2" s="1"/>
-      <c r="BS2" s="1"/>
-      <c r="BT2" s="1"/>
-      <c r="BU2" s="1"/>
-      <c r="BV2" s="1"/>
-      <c r="BW2" s="1"/>
-      <c r="BX2" s="1"/>
-      <c r="BY2" s="1"/>
-      <c r="BZ2" s="1"/>
-      <c r="CA2" s="1"/>
-      <c r="CB2" s="1"/>
-      <c r="CC2" s="1"/>
-      <c r="CD2" s="1"/>
-      <c r="CE2" s="1"/>
-      <c r="CF2" s="1"/>
-      <c r="CG2" s="1"/>
-      <c r="CH2" s="1"/>
-      <c r="CI2" s="1"/>
+    <row r="2" spans="1:99" s="2" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="16"/>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="16"/>
+      <c r="AN2" s="16"/>
+      <c r="AO2" s="16"/>
+      <c r="AP2" s="16"/>
+      <c r="AQ2" s="16"/>
+      <c r="AR2" s="16"/>
+      <c r="AS2" s="16"/>
+      <c r="AT2" s="16"/>
+      <c r="AU2" s="16"/>
+      <c r="AV2" s="16"/>
+      <c r="AW2" s="16"/>
+      <c r="AX2" s="16"/>
+      <c r="AY2" s="16"/>
+      <c r="AZ2" s="16"/>
+      <c r="BA2" s="16"/>
+      <c r="BB2" s="16"/>
+      <c r="BC2" s="16"/>
+      <c r="BD2" s="16"/>
+      <c r="BE2" s="16"/>
+      <c r="BF2" s="16"/>
+      <c r="BG2" s="16"/>
+      <c r="BH2" s="16"/>
+      <c r="BI2" s="16"/>
+      <c r="BJ2" s="16"/>
+      <c r="BK2" s="16"/>
+      <c r="BL2" s="16"/>
+      <c r="BM2" s="16"/>
+      <c r="BN2" s="16"/>
+      <c r="BO2" s="16"/>
+      <c r="BP2" s="16"/>
+      <c r="BQ2" s="16"/>
+      <c r="BR2" s="16"/>
+      <c r="BS2" s="16"/>
+      <c r="BT2" s="16"/>
+      <c r="BU2" s="16"/>
+      <c r="BV2" s="16"/>
+      <c r="BW2" s="16"/>
+      <c r="BX2" s="16"/>
+      <c r="BY2" s="16"/>
+      <c r="BZ2" s="16"/>
+      <c r="CA2" s="16"/>
+      <c r="CB2" s="16"/>
+      <c r="CC2" s="16"/>
+      <c r="CD2" s="16"/>
+      <c r="CE2" s="16"/>
+      <c r="CF2" s="16"/>
+      <c r="CG2" s="16"/>
+      <c r="CH2" s="16"/>
+      <c r="CI2" s="16"/>
+      <c r="CJ2" s="16"/>
+      <c r="CK2" s="16"/>
+      <c r="CL2" s="16"/>
+      <c r="CM2" s="16"/>
+      <c r="CN2" s="17"/>
+      <c r="CO2" s="17"/>
+      <c r="CP2" s="17"/>
+      <c r="CQ2" s="17"/>
+      <c r="CR2" s="17"/>
+      <c r="CS2" s="17"/>
+      <c r="CT2" s="17"/>
+      <c r="CU2" s="17"/>
     </row>
-    <row r="6" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="M2:CH2"/>
+  <autoFilter ref="M2:CU2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>